<commit_message>
Cập nhật toàn bộ tên liên lạc = 'Juan' cho những khách hàng ở Mexico : UPDATE Customers SET ContactName = 'Juan' WHERE Country = 'Mexico'
</commit_message>
<xml_diff>
--- a/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
+++ b/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
@@ -377,6 +377,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="22"/>
       <color rgb="FF000000"/>
@@ -392,12 +398,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -530,19 +530,19 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
@@ -551,28 +551,28 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="7" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
@@ -582,7 +582,7 @@
       <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1370,7 +1370,7 @@
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="126.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="121.5" customFormat="1" s="1">
       <c r="A17" s="7"/>
       <c r="B17" s="13">
         <v>13</v>
@@ -1399,7 +1399,7 @@
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="49.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="34.5" customFormat="1" s="1">
       <c r="A18" s="7"/>
       <c r="B18" s="13">
         <v>14</v>

</xml_diff>

<commit_message>
Lấy trung bình giá của sản phẩm :  SELECT AVG (Price) FROM Products
</commit_message>
<xml_diff>
--- a/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
+++ b/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
@@ -1506,7 +1506,7 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="44.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="34.5" customFormat="1" s="1">
       <c r="A22" s="2"/>
       <c r="B22" s="12">
         <v>18</v>
@@ -1535,7 +1535,7 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="39.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="34.5" customFormat="1" s="1">
       <c r="A23" s="2"/>
       <c r="B23" s="12">
         <v>19</v>

</xml_diff>

<commit_message>
Lọc ra những sản phẩm có giá từ 40 đến 90 ( lấy những sản phẩm có giá = 40 và = 90) :  SELECT * FROM Products WHERE Price >= 40 AND Price <= 90
</commit_message>
<xml_diff>
--- a/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
+++ b/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
@@ -2260,7 +2260,7 @@
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="123.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="121.5" customFormat="1" s="1">
       <c r="A48" s="2"/>
       <c r="B48" s="12">
         <v>44</v>
@@ -2289,7 +2289,7 @@
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="69" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="64.5" customFormat="1" s="1">
       <c r="A49" s="2"/>
       <c r="B49" s="12">
         <v>45</v>
@@ -2318,7 +2318,7 @@
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="15.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A50" s="2"/>
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
@@ -2341,7 +2341,7 @@
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="15.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A51" s="2"/>
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
@@ -2364,7 +2364,7 @@
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="15.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A52" s="2"/>
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
@@ -2387,7 +2387,7 @@
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="15.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A53" s="2"/>
       <c r="B53" s="7"/>
       <c r="C53" s="8"/>
@@ -2410,7 +2410,7 @@
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="15.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A54" s="2"/>
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
@@ -2433,7 +2433,7 @@
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="15.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A55" s="2"/>
       <c r="B55" s="7"/>
       <c r="C55" s="8"/>
@@ -2456,7 +2456,7 @@
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="15.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A56" s="2"/>
       <c r="B56" s="7"/>
       <c r="C56" s="8"/>
@@ -2479,7 +2479,7 @@
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="15.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A57" s="2"/>
       <c r="B57" s="7"/>
       <c r="C57" s="8"/>

</xml_diff>

<commit_message>
Lọc ra danh sách tên khách hàng, tên liên lạc của khách hàng và lưu vào 1 bảng mới :   CREATE TABLE NEWTABLE AS   SELECT CustomerName, ContactName    FROM CUSTOMERS
</commit_message>
<xml_diff>
--- a/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
+++ b/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
@@ -1622,7 +1622,7 @@
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="55.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="49.5" customFormat="1" s="1">
       <c r="A26" s="2"/>
       <c r="B26" s="12">
         <v>22</v>
@@ -1651,7 +1651,7 @@
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="56.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="49.5" customFormat="1" s="1">
       <c r="A27" s="2"/>
       <c r="B27" s="12">
         <v>23</v>

</xml_diff>

<commit_message>
Lấy ra tên sản phẩm có giá cao nhất trong bảng :    SELECT MAX(Price) AS MaxPrice, ProductName FROM Products ORDER BY ProductName
</commit_message>
<xml_diff>
--- a/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
+++ b/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
@@ -1767,7 +1767,7 @@
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="41.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A31" s="2"/>
       <c r="B31" s="12">
         <v>27</v>
@@ -1796,7 +1796,7 @@
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="84.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="78" customFormat="1" s="1">
       <c r="A32" s="2"/>
       <c r="B32" s="12">
         <v>28</v>
@@ -1825,7 +1825,7 @@
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="45.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A33" s="2"/>
       <c r="B33" s="12">
         <v>29</v>
@@ -1854,7 +1854,7 @@
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="71.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="61.5" customFormat="1" s="1">
       <c r="A34" s="2"/>
       <c r="B34" s="12">
         <v>30</v>
@@ -1883,7 +1883,7 @@
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="48.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A35" s="2"/>
       <c r="B35" s="12">
         <v>31</v>

</xml_diff>

<commit_message>
Lấy ra danh sách city ở khách hàng và nhà cung cấp rồi sắp xếp theo thứ tự tăng dần :    SELECT Customers.City, Suppliers.City FROM Customers,    Suppliers ORDER BY Customers.City, Suppliers.City DESC
</commit_message>
<xml_diff>
--- a/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
+++ b/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
@@ -1680,7 +1680,7 @@
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="108" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="102.75" customFormat="1" s="1">
       <c r="A28" s="2"/>
       <c r="B28" s="12">
         <v>24</v>
@@ -1709,7 +1709,7 @@
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="63.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="61.5" customFormat="1" s="1">
       <c r="A29" s="2"/>
       <c r="B29" s="12">
         <v>25</v>

</xml_diff>

<commit_message>
Lấy ra toàn bộ danh sách họ tên nhân viên và mã đơn hàng họ đặt được (nếu có) : SELECT Employees.LastName, Employees.FirstName, Orders.OrderID FROM Employees JOIN Orders ON Employees.EmployeeID=Orders.EmployeeID
</commit_message>
<xml_diff>
--- a/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
+++ b/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
@@ -1999,7 +1999,7 @@
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="53.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="49.5" customFormat="1" s="1">
       <c r="A39" s="2"/>
       <c r="B39" s="12">
         <v>35</v>
@@ -2028,7 +2028,7 @@
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="67.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="63.75" customFormat="1" s="1">
       <c r="A40" s="2"/>
       <c r="B40" s="12">
         <v>36</v>

</xml_diff>

<commit_message>
Lấy ra id khách hàng order trên 6 đơn : SELECT Orders.CustomerID, OrderDetails. Quantity FROM OrderDetails JOIN Orders ON OrderDetails.OrderID=Orders.OrderID WHERE OrderDetails.Quantity > 6 GROUP BY Orders.CustomerID
</commit_message>
<xml_diff>
--- a/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
+++ b/SQL-Basic/5.3 BÀI TẬP THỰC HÀNH SQL  TRÊN W3C.xlsx
@@ -2057,7 +2057,7 @@
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="63.75" customFormat="1" s="1">
       <c r="A41" s="2"/>
       <c r="B41" s="12">
         <v>37</v>
@@ -2086,7 +2086,7 @@
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="83.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="78" customFormat="1" s="1">
       <c r="A42" s="2"/>
       <c r="B42" s="12">
         <v>38</v>

</xml_diff>